<commit_message>
reformatting the segment meta data
</commit_message>
<xml_diff>
--- a/--- meta-data-formation/Template_for_data_deadline_stress.xlsx
+++ b/--- meta-data-formation/Template_for_data_deadline_stress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shailazaman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shailazaman/Google Drive/University of Houston/CS - UH/@Research - CPL/@CPL-Projects/DealineStressDataAnalysis/--- meta-data-formation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC50ADF-B2A1-E84C-9A01-06E811B3B30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7DD49C-9A78-1D45-96B5-93EBE297E3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22480" windowHeight="16620" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="18580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>Participant_ID</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>PSYCHOMETRICS…All</t>
-  </si>
-  <si>
-    <t>segment start time-end time</t>
   </si>
 </sst>
 </file>
@@ -752,10 +749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,19 +765,18 @@
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,37 +802,34 @@
         <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>30</v>
       </c>
@@ -846,14 +839,14 @@
       <c r="H2">
         <v>523</v>
       </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
       <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>30</v>
       </c>
@@ -863,14 +856,14 @@
       <c r="H3">
         <v>454</v>
       </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
       <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>30</v>
       </c>
@@ -880,10 +873,10 @@
       <c r="H4">
         <v>323</v>
       </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
       <c r="K4">
-        <v>3</v>
-      </c>
-      <c r="L4">
         <v>14</v>
       </c>
     </row>

</xml_diff>